<commit_message>
Daily attendance processing - 2025-09-18 03:31:29
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_Pediatrics_attendance.xlsx
+++ b/attendance_reports/Y4_B2526_Pediatrics_attendance.xlsx
@@ -559,22 +559,22 @@
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>Required pediatrics (Total)</t>
+          <t>Required PEDIATRICS (Total)</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Attended pediatrics (Total)</t>
+          <t>Attended PEDIATRICS (Total)</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
         <is>
-          <t>pediatrics S1 (Req)</t>
+          <t>PEDIATRICS S1 (Req)</t>
         </is>
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>pediatrics S1 (Att)</t>
+          <t>PEDIATRICS S1 (Att)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-24 18:31:06
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_Pediatrics_attendance.xlsx
+++ b/attendance_reports/Y4_B2526_Pediatrics_attendance.xlsx
@@ -7,14 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary_updated" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Attendance_updated" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Transfers_updated" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Attendance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Transfers" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary_updated'!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance_updated'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Transfers_updated'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Transfers'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -87915,7 +87915,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -87932,6 +87932,7 @@
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
@@ -87965,9 +87966,14 @@
           <t>Transfer Date</t>
         </is>
       </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>